<commit_message>
conversations history is now working
</commit_message>
<xml_diff>
--- a/kalkulation projectGPT.xlsx
+++ b/kalkulation projectGPT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohaalsalatini/Desktop/Projekte/Cloudpioneer/AI-ProjectChat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8677FAE9-7B95-894E-9730-F9E2AA4D2D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF91559-ADDF-0E43-A800-66A2BA57E33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-480" windowWidth="38400" windowHeight="20980" xr2:uid="{38BF9AA1-F641-3346-957F-2790587D94D9}"/>
   </bookViews>
@@ -407,7 +407,7 @@
   <dimension ref="A2:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>